<commit_message>
Add README, Change image storage strategy from static folder to MongoDB
</commit_message>
<xml_diff>
--- a/Byarent User Stories.xlsx
+++ b/Byarent User Stories.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Table 1</t>
   </si>
@@ -63,7 +70,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -82,7 +89,7 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -99,7 +106,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -116,9 +123,42 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="1"/>
+    <t xml:space="preserve">add new houses, </t>
+  </si>
+  <si>
+    <t>sell them to site users</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The Admin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Should</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> be able to add new houses</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -131,11 +171,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t xml:space="preserve">: Not started, </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
+      <t xml:space="preserve">: Create and Order models and routes that store all existing data on houses to be sold and orders made by users </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -148,14 +188,14 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>: Not started</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">add new houses, </t>
-  </si>
-  <si>
-    <t>sell them to site users</t>
+      <t>: Make available in a simple and straightforward manner all existing data on houses and orders</t>
+    </r>
+  </si>
+  <si>
+    <t>edit existing houses</t>
+  </si>
+  <si>
+    <t>more accurately and appealingly portray them to site users</t>
   </si>
   <si>
     <r>
@@ -168,26 +208,148 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Should</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> be able to add new houses</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Should be able to edit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>existing</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>houses</t>
+    </r>
+  </si>
+  <si>
+    <t>delete existing houses once they are sold</t>
+  </si>
+  <si>
+    <t>only show users houses that are available</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> The Admin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Should </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>be able to delete houses</t>
+    </r>
+  </si>
+  <si>
+    <t>view orders received</t>
+  </si>
+  <si>
+    <t>follow up the orders</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> The Admin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Should </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>be able to view orders received</t>
+    </r>
+  </si>
+  <si>
+    <t>Customer View</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>view all the houses on sale</t>
+  </si>
+  <si>
+    <t>select one that I prefer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>The User S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>hould</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> be able to view the houses on sale without having to login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -200,11 +362,11 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t xml:space="preserve">: Create and Order models and routes that store all existing data on houses to be sold and orders made by users </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
+      <t xml:space="preserve">: Fetch data on all existing houses that haven't been sold. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -217,13 +379,49 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>: Make available in a simple and straightforward manner all existing data on houses and orders</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
+      <t>: Display the houses on sale with a simple, interactive and aesthetically pleasing UI</t>
+    </r>
+  </si>
+  <si>
+    <t>Login &amp; Signup</t>
+  </si>
+  <si>
+    <t>make an account</t>
+  </si>
+  <si>
+    <t>be able to place orders</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> have a signup page that takes in their email and password, and names</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -236,11 +434,257 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
+      <t xml:space="preserve">: Create a user model containing all user info, implement password encryption on signup and authentication on login. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Frontend: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Make the signup and login pages simple and straightforward</t>
+    </r>
+  </si>
+  <si>
+    <t>sign in to my account</t>
+  </si>
+  <si>
+    <t>Shopping Cart</t>
+  </si>
+  <si>
+    <t>make an order</t>
+  </si>
+  <si>
+    <t>rent the house I prefer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> be able to make orders</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: All orders placed should be stored in session storage and made accessible in a shopping cart until they are checked out, when they can be allowed to affect the database. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Frontend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>: All orders made should be easily accessible in a shopping cart</t>
+    </r>
+  </si>
+  <si>
+    <t>undo an order</t>
+  </si>
+  <si>
+    <t>choose a different house</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> be able to undo orders</t>
+    </r>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">The User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> be able to logout</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: The User session should persist using session storage until dismissed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Frontend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>: The logout button should be easily accessible without being an eyesore</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">: Done, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Frontend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>: Done</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>Backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
       <t xml:space="preserve">: Complete, </t>
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -253,455 +697,15 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>: Not started</t>
-    </r>
-  </si>
-  <si>
-    <t>edit existing houses</t>
-  </si>
-  <si>
-    <t>more accurately and appealingly portray them to site users</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The Admin </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">Should be able to edit </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>existing</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>houses</t>
-    </r>
-  </si>
-  <si>
-    <t>delete existing houses once they are sold</t>
-  </si>
-  <si>
-    <t>only show users houses that are available</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> The Admin </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">Should </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>be able to delete houses</t>
-    </r>
-  </si>
-  <si>
-    <t>view orders received</t>
-  </si>
-  <si>
-    <t>follow up the orders</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> The Admin </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">Should </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>be able to view orders received</t>
-    </r>
-  </si>
-  <si>
-    <t>Customer View</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>view all the houses on sale</t>
-  </si>
-  <si>
-    <t>select one that I prefer</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>The User S</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>hould</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> be able to view the houses on sale without having to login</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Backend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">: Fetch data on all existing houses that haven't been sold. </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Frontend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>: Display the houses on sale with a simple, interactive and aesthetically pleasing UI</t>
-    </r>
-  </si>
-  <si>
-    <t>Login &amp; Signup</t>
-  </si>
-  <si>
-    <t>make an account</t>
-  </si>
-  <si>
-    <t>be able to place orders</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The User </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> have a signup page that takes in their email and password, and names</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Backend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">: Create a user model containing all user info, implement password encryption on signup and authentication on login. </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">Frontend: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Make the signup and login pages simple and straightforward</t>
-    </r>
-  </si>
-  <si>
-    <t>sign in to my account</t>
-  </si>
-  <si>
-    <t>Shopping Cart</t>
-  </si>
-  <si>
-    <t>make an order</t>
-  </si>
-  <si>
-    <t>rent the house I prefer</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The User </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> be able to make orders</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Backend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">: All orders placed should be stored in session storage and made accessible in a shopping cart until they are checked out, when they can be allowed to affect the database. </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Frontend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>: All orders made should be easily accessible in a shopping cart</t>
-    </r>
-  </si>
-  <si>
-    <t>undo an order</t>
-  </si>
-  <si>
-    <t>choose a different house</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The User </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> be able to undo orders</t>
-    </r>
-  </si>
-  <si>
-    <t>logout</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">The User </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve"> be able to logout</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Backend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">: The User session should persist using session storage until dismissed. </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Frontend</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>: The logout button should be easily accessible without being an eyesore</t>
+      <t>: Done</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -718,7 +722,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -769,33 +773,39 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -803,27 +813,80 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="001FB714"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1015,7 +1078,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1024,7 +1087,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1033,7 +1096,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1042,7 +1105,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1051,7 +1114,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1060,7 +1123,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1172,8 +1235,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -1181,14 +1244,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1207,7 +1270,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1278,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -1243,7 +1306,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1269,7 +1332,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1295,7 +1358,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1321,7 +1384,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1347,7 +1410,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1373,7 +1436,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1399,7 +1462,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1425,7 +1488,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1451,7 +1514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1464,9 +1527,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1482,7 +1551,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1501,7 +1570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1527,7 +1596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1553,7 +1622,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1579,7 +1648,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1605,7 +1674,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1631,7 +1700,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1657,7 +1726,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1683,7 +1752,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1709,7 +1778,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1735,7 +1804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1748,9 +1817,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1763,7 +1838,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1782,7 +1857,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1812,7 +1887,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1838,7 +1913,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1864,7 +1939,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1890,7 +1965,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1916,7 +1991,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1942,7 +2017,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1968,7 +2043,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1994,7 +2069,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2020,7 +2095,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2033,552 +2108,557 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K26"/>
+  <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="D3" xSplit="3" ySplit="2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F8" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.8828" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.8828" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.8828" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1562" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.9141" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.9531" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.4844" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.9297" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.05469" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.05469" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.05469" style="1" customWidth="1"/>
-    <col min="12" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="1" max="3" width="13.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.875" style="1" customWidth="1"/>
+    <col min="9" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:11" ht="16">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
-    <row r="2" ht="32.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:11" ht="32.5" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" ht="80.55" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" spans="1:11" ht="80.5" customHeight="1">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s" s="5">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="5">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s" s="5">
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
-    <row r="4" ht="32.35" customHeight="1">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s" s="4">
+    <row r="5" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s" s="5">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s" s="5">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
-    <row r="5" ht="32.35" customHeight="1">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="4">
+    <row r="6" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s" s="5">
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s" s="5">
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
-    <row r="6" ht="32.35" customHeight="1">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s" s="4">
+    <row r="7" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s" s="5">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s" s="5">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
     </row>
-    <row r="7" ht="32.35" customHeight="1">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s" s="4">
+    <row r="8" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="56.25" customHeight="1">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="35.75" customHeight="1">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="32.5" customHeight="1">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" customHeight="1">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="D7" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s" s="5">
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
+      <c r="D13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
+    <row r="14" spans="1:11" ht="56.25" customHeight="1">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
-    <row r="9" ht="56.35" customHeight="1">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s" s="4">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s" s="5">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s" s="5">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+    <row r="15" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
-    <row r="10" ht="35.75" customHeight="1">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s" s="5">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s" s="5">
-        <v>40</v>
-      </c>
-      <c r="H10" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
+    <row r="16" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
-    <row r="11" ht="32.55" customHeight="1">
-      <c r="A11" s="4">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s" s="5">
-        <v>38</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
+    <row r="17" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
-    <row r="12" ht="32.35" customHeight="1">
-      <c r="A12" s="4">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s" s="5">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s" s="5">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="H12" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+    <row r="18" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
     </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="4">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s" s="4">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D13" t="s" s="5">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s" s="5">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s" s="5">
-        <v>49</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+    <row r="19" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
     </row>
-    <row r="14" ht="56.35" customHeight="1">
-      <c r="A14" s="4">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s" s="4">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s" s="5">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s" s="5">
-        <v>52</v>
-      </c>
-      <c r="H14" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+    <row r="20" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
     </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+    <row r="21" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+    <row r="22" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
     </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+    <row r="23" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
     </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+    <row r="24" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+    <row r="25" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+    <row r="26" spans="1:11" ht="20.25" customHeight="1">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2592,9 +2672,13 @@
     <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>